<commit_message>
envios y arreglo del serviciosInternos movile y checkbox
</commit_message>
<xml_diff>
--- a/backend/data/frente_alto.xlsx
+++ b/backend/data/frente_alto.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -454,9 +454,61 @@
         <v>28/5/2025, 7:48:12 p.m.</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Luciano</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Albani</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Mar del Plata</v>
+      </c>
+      <c r="D3" t="str">
+        <v>luchoalbanix1@gmail.com</v>
+      </c>
+      <c r="E3" t="str">
+        <v>+54 2234480301</v>
+      </c>
+      <c r="F3" t="str">
+        <v>rango4</v>
+      </c>
+      <c r="G3" t="str">
+        <v>En un mes</v>
+      </c>
+      <c r="H3" t="str">
+        <v>31/5/2025, 1:49:42 a.m.</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Luciano</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Albani</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Mar del Plata</v>
+      </c>
+      <c r="D4" t="str">
+        <v>luchoalbanix1@gmail.com</v>
+      </c>
+      <c r="E4" t="str">
+        <v>+1242 2234480301</v>
+      </c>
+      <c r="F4" t="str">
+        <v>rango5</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Inmediatamente</v>
+      </c>
+      <c r="H4" t="str">
+        <v>31/5/2025, 3:15:56 a.m.</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>